<commit_message>
correct ihe profiles 867d463029a308f0bd25b6431988891963d03411
</commit_message>
<xml_diff>
--- a/ig/nr/correctErrors/StructureDefinition-pdsm-simplified-publish.xlsx
+++ b/ig/nr/correctErrors/StructureDefinition-pdsm-simplified-publish.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-20T10:43:12+00:00</t>
+    <t>2023-03-20T10:49:37+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1612,7 +1612,7 @@
 constr-bind-ProducteurDoc-simplified:L’utilisation de cette nomenclature est recommandée mais non obligatoire (prefered) :
 -	TRE_R02-SecteurActivite, OID : 1.2.250.1.71.4.2.4 (lorsque l’auteur du document est un professionnel ou un équipement sous sa responsabilité)
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J61-HealthcareFacilityTypeCode-DMP).
-En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J02-XdsHealthcareFacilityTypeCode-CISIS peut être utilisé. {null}</t>
+En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J02-XdsHealthcareFacilityTypeCode-CISIS peut être utilisé. {f:context/f:practiceSetting or f:context/f:facilityType}</t>
   </si>
   <si>
     <t>usually from a mapping to a local ValueSet</t>

</xml_diff>